<commit_message>
Massive improvement in the resampling functions, From 68ms to 300us
</commit_message>
<xml_diff>
--- a/profiler/Comparison.xlsx
+++ b/profiler/Comparison.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CImplData" sheetId="1" r:id="rId1"/>
-    <sheet name="CImplStats" sheetId="2" r:id="rId2"/>
-    <sheet name="CUDA1Data" sheetId="3" r:id="rId3"/>
+    <sheet name="CUDA1Data" sheetId="3" r:id="rId2"/>
+    <sheet name="CImplStats" sheetId="2" r:id="rId3"/>
     <sheet name="CUDA1Stats" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -32614,318 +32614,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="A1:E14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="str">
-        <f>LOOKUP($A2,CImplData!$C:$C,CImplData!B:B)</f>
-        <v>Generating weights</v>
-      </c>
-      <c r="C2">
-        <f>COUNTIF(CImplData!$C:$C, $A2)</f>
-        <v>200</v>
-      </c>
-      <c r="D2">
-        <f>AVERAGEIF(CImplData!$C:$C,A2,CImplData!$F:$F)</f>
-        <v>531.7014949999998</v>
-      </c>
-      <c r="E2" t="str">
-        <f>LOOKUP($A2,CImplData!$C:$C,CImplData!$A:$A)</f>
-        <v>#FF00FF00</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="str">
-        <f>LOOKUP($A3,CImplData!$C:$C,CImplData!B:B)</f>
-        <v>Normalizing</v>
-      </c>
-      <c r="C3">
-        <f>COUNTIF(CImplData!$C:$C, $A3)</f>
-        <v>200</v>
-      </c>
-      <c r="D3">
-        <f>AVERAGEIF(CImplData!$C:$C,A3,CImplData!$F:$F)</f>
-        <v>5.7428249999999981</v>
-      </c>
-      <c r="E3" t="str">
-        <f>LOOKUP($A3,CImplData!$C:$C,CImplData!$A:$A)</f>
-        <v>#FF0000FF</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="str">
-        <f>LOOKUP($A4,CImplData!$C:$C,CImplData!B:B)</f>
-        <v>Resampling</v>
-      </c>
-      <c r="C4">
-        <f>COUNTIF(CImplData!$C:$C, $A4)</f>
-        <v>200</v>
-      </c>
-      <c r="D4">
-        <f>AVERAGEIF(CImplData!$C:$C,A4,CImplData!$F:$F)</f>
-        <v>19041.365895000003</v>
-      </c>
-      <c r="E4" t="str">
-        <f>LOOKUP($A4,CImplData!$C:$C,CImplData!$A:$A)</f>
-        <v>#FF00FFFF</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="str">
-        <f>LOOKUP($A5,CImplData!$C:$C,CImplData!B:B)</f>
-        <v>Resampling</v>
-      </c>
-      <c r="C5">
-        <f>COUNTIF(CImplData!$C:$C, $A5)</f>
-        <v>0</v>
-      </c>
-      <c r="D5" t="e">
-        <f>AVERAGEIF(CImplData!$C:$C,A5,CImplData!$F:$F)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E5" t="str">
-        <f>LOOKUP($A5,CImplData!$C:$C,CImplData!$A:$A)</f>
-        <v>#FF00FFFF</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="str">
-        <f>LOOKUP($A6,CImplData!$C:$C,CImplData!B:B)</f>
-        <v>Resampling</v>
-      </c>
-      <c r="C6">
-        <f>COUNTIF(CImplData!$C:$C, $A6)</f>
-        <v>0</v>
-      </c>
-      <c r="D6" t="e">
-        <f>AVERAGEIF(CImplData!$C:$C,A6,CImplData!$F:$F)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E6" t="str">
-        <f>LOOKUP($A6,CImplData!$C:$C,CImplData!$A:$A)</f>
-        <v>#FF00FFFF</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="str">
-        <f>LOOKUP($A7,CImplData!$C:$C,CImplData!B:B)</f>
-        <v>Resampling</v>
-      </c>
-      <c r="C7">
-        <f>COUNTIF(CImplData!$C:$C, $A7)</f>
-        <v>0</v>
-      </c>
-      <c r="D7" t="e">
-        <f>AVERAGEIF(CImplData!$C:$C,A7,CImplData!$F:$F)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E7" t="str">
-        <f>LOOKUP($A7,CImplData!$C:$C,CImplData!$A:$A)</f>
-        <v>#FF00FFFF</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="str">
-        <f>LOOKUP($A8,CImplData!$C:$C,CImplData!B:B)</f>
-        <v>Resampling</v>
-      </c>
-      <c r="C8">
-        <f>COUNTIF(CImplData!$C:$C, $A8)</f>
-        <v>0</v>
-      </c>
-      <c r="D8" t="e">
-        <f>AVERAGEIF(CImplData!$C:$C,A8,CImplData!$F:$F)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E8" t="str">
-        <f>LOOKUP($A8,CImplData!$C:$C,CImplData!$A:$A)</f>
-        <v>#FF00FFFF</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="str">
-        <f>LOOKUP($A9,CImplData!$C:$C,CImplData!B:B)</f>
-        <v>Resampling</v>
-      </c>
-      <c r="C9">
-        <f>COUNTIF(CImplData!$C:$C, $A9)</f>
-        <v>0</v>
-      </c>
-      <c r="D9" t="e">
-        <f>AVERAGEIF(CImplData!$C:$C,A9,CImplData!$F:$F)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E9" t="str">
-        <f>LOOKUP($A9,CImplData!$C:$C,CImplData!$A:$A)</f>
-        <v>#FF00FFFF</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="str">
-        <f>LOOKUP($A10,CImplData!$C:$C,CImplData!B:B)</f>
-        <v>Resampling</v>
-      </c>
-      <c r="C10">
-        <f>COUNTIF(CImplData!$C:$C, $A10)</f>
-        <v>0</v>
-      </c>
-      <c r="D10" t="e">
-        <f>AVERAGEIF(CImplData!$C:$C,A10,CImplData!$F:$F)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E10" t="str">
-        <f>LOOKUP($A10,CImplData!$C:$C,CImplData!$A:$A)</f>
-        <v>#FF00FFFF</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="str">
-        <f>LOOKUP($A11,CImplData!$C:$C,CImplData!B:B)</f>
-        <v>Resampling</v>
-      </c>
-      <c r="C11">
-        <f>COUNTIF(CImplData!$C:$C, $A11)</f>
-        <v>0</v>
-      </c>
-      <c r="D11" t="e">
-        <f>AVERAGEIF(CImplData!$C:$C,A11,CImplData!$F:$F)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E11" t="str">
-        <f>LOOKUP($A11,CImplData!$C:$C,CImplData!$A:$A)</f>
-        <v>#FF00FFFF</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="str">
-        <f>LOOKUP($A12,CImplData!$C:$C,CImplData!B:B)</f>
-        <v>Resampling</v>
-      </c>
-      <c r="C12">
-        <f>COUNTIF(CImplData!$C:$C, $A12)</f>
-        <v>0</v>
-      </c>
-      <c r="D12" t="e">
-        <f>AVERAGEIF(CImplData!$C:$C,A12,CImplData!$F:$F)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E12" t="str">
-        <f>LOOKUP($A12,CImplData!$C:$C,CImplData!$A:$A)</f>
-        <v>#FF00FFFF</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="str">
-        <f>LOOKUP($A13,CImplData!$C:$C,CImplData!B:B)</f>
-        <v>Resampling</v>
-      </c>
-      <c r="C13">
-        <f>COUNTIF(CImplData!$C:$C, $A13)</f>
-        <v>0</v>
-      </c>
-      <c r="D13" t="e">
-        <f>AVERAGEIF(CImplData!$C:$C,A13,CImplData!$F:$F)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E13" t="str">
-        <f>LOOKUP($A13,CImplData!$C:$C,CImplData!$A:$A)</f>
-        <v>#FF00FFFF</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="str">
-        <f>LOOKUP($A14,CImplData!$C:$C,CImplData!B:B)</f>
-        <v>Resampling</v>
-      </c>
-      <c r="C14">
-        <f>COUNTIF(CImplData!$C:$C, $A14)</f>
-        <v>0</v>
-      </c>
-      <c r="D14" t="e">
-        <f>AVERAGEIF(CImplData!$C:$C,A14,CImplData!$F:$F)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E14" t="str">
-        <f>LOOKUP($A14,CImplData!$C:$C,CImplData!$A:$A)</f>
-        <v>#FF00FFFF</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q406"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -54457,11 +54145,323 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="OL1" workbookViewId="0">
+      <selection activeCell="D4" sqref="A1:E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <f>LOOKUP($A2,CImplData!$C:$C,CImplData!B:B)</f>
+        <v>Generating weights</v>
+      </c>
+      <c r="C2">
+        <f>COUNTIF(CImplData!$C:$C, $A2)</f>
+        <v>200</v>
+      </c>
+      <c r="D2">
+        <f>AVERAGEIF(CImplData!$C:$C,A2,CImplData!$F:$F)</f>
+        <v>531.7014949999998</v>
+      </c>
+      <c r="E2" t="str">
+        <f>LOOKUP($A2,CImplData!$C:$C,CImplData!$A:$A)</f>
+        <v>#FF00FF00</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f>LOOKUP($A3,CImplData!$C:$C,CImplData!B:B)</f>
+        <v>Normalizing</v>
+      </c>
+      <c r="C3">
+        <f>COUNTIF(CImplData!$C:$C, $A3)</f>
+        <v>200</v>
+      </c>
+      <c r="D3">
+        <f>AVERAGEIF(CImplData!$C:$C,A3,CImplData!$F:$F)</f>
+        <v>5.7428249999999981</v>
+      </c>
+      <c r="E3" t="str">
+        <f>LOOKUP($A3,CImplData!$C:$C,CImplData!$A:$A)</f>
+        <v>#FF0000FF</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f>LOOKUP($A4,CImplData!$C:$C,CImplData!B:B)</f>
+        <v>Resampling</v>
+      </c>
+      <c r="C4">
+        <f>COUNTIF(CImplData!$C:$C, $A4)</f>
+        <v>200</v>
+      </c>
+      <c r="D4">
+        <f>AVERAGEIF(CImplData!$C:$C,A4,CImplData!$F:$F)</f>
+        <v>19041.365895000003</v>
+      </c>
+      <c r="E4" t="str">
+        <f>LOOKUP($A4,CImplData!$C:$C,CImplData!$A:$A)</f>
+        <v>#FF00FFFF</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f>LOOKUP($A5,CImplData!$C:$C,CImplData!B:B)</f>
+        <v>Resampling</v>
+      </c>
+      <c r="C5">
+        <f>COUNTIF(CImplData!$C:$C, $A5)</f>
+        <v>0</v>
+      </c>
+      <c r="D5" t="e">
+        <f>AVERAGEIF(CImplData!$C:$C,A5,CImplData!$F:$F)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E5" t="str">
+        <f>LOOKUP($A5,CImplData!$C:$C,CImplData!$A:$A)</f>
+        <v>#FF00FFFF</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <f>LOOKUP($A6,CImplData!$C:$C,CImplData!B:B)</f>
+        <v>Resampling</v>
+      </c>
+      <c r="C6">
+        <f>COUNTIF(CImplData!$C:$C, $A6)</f>
+        <v>0</v>
+      </c>
+      <c r="D6" t="e">
+        <f>AVERAGEIF(CImplData!$C:$C,A6,CImplData!$F:$F)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E6" t="str">
+        <f>LOOKUP($A6,CImplData!$C:$C,CImplData!$A:$A)</f>
+        <v>#FF00FFFF</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <f>LOOKUP($A7,CImplData!$C:$C,CImplData!B:B)</f>
+        <v>Resampling</v>
+      </c>
+      <c r="C7">
+        <f>COUNTIF(CImplData!$C:$C, $A7)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" t="e">
+        <f>AVERAGEIF(CImplData!$C:$C,A7,CImplData!$F:$F)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E7" t="str">
+        <f>LOOKUP($A7,CImplData!$C:$C,CImplData!$A:$A)</f>
+        <v>#FF00FFFF</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <f>LOOKUP($A8,CImplData!$C:$C,CImplData!B:B)</f>
+        <v>Resampling</v>
+      </c>
+      <c r="C8">
+        <f>COUNTIF(CImplData!$C:$C, $A8)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" t="e">
+        <f>AVERAGEIF(CImplData!$C:$C,A8,CImplData!$F:$F)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E8" t="str">
+        <f>LOOKUP($A8,CImplData!$C:$C,CImplData!$A:$A)</f>
+        <v>#FF00FFFF</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <f>LOOKUP($A9,CImplData!$C:$C,CImplData!B:B)</f>
+        <v>Resampling</v>
+      </c>
+      <c r="C9">
+        <f>COUNTIF(CImplData!$C:$C, $A9)</f>
+        <v>0</v>
+      </c>
+      <c r="D9" t="e">
+        <f>AVERAGEIF(CImplData!$C:$C,A9,CImplData!$F:$F)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E9" t="str">
+        <f>LOOKUP($A9,CImplData!$C:$C,CImplData!$A:$A)</f>
+        <v>#FF00FFFF</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <f>LOOKUP($A10,CImplData!$C:$C,CImplData!B:B)</f>
+        <v>Resampling</v>
+      </c>
+      <c r="C10">
+        <f>COUNTIF(CImplData!$C:$C, $A10)</f>
+        <v>0</v>
+      </c>
+      <c r="D10" t="e">
+        <f>AVERAGEIF(CImplData!$C:$C,A10,CImplData!$F:$F)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E10" t="str">
+        <f>LOOKUP($A10,CImplData!$C:$C,CImplData!$A:$A)</f>
+        <v>#FF00FFFF</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <f>LOOKUP($A11,CImplData!$C:$C,CImplData!B:B)</f>
+        <v>Resampling</v>
+      </c>
+      <c r="C11">
+        <f>COUNTIF(CImplData!$C:$C, $A11)</f>
+        <v>0</v>
+      </c>
+      <c r="D11" t="e">
+        <f>AVERAGEIF(CImplData!$C:$C,A11,CImplData!$F:$F)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E11" t="str">
+        <f>LOOKUP($A11,CImplData!$C:$C,CImplData!$A:$A)</f>
+        <v>#FF00FFFF</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="str">
+        <f>LOOKUP($A12,CImplData!$C:$C,CImplData!B:B)</f>
+        <v>Resampling</v>
+      </c>
+      <c r="C12">
+        <f>COUNTIF(CImplData!$C:$C, $A12)</f>
+        <v>0</v>
+      </c>
+      <c r="D12" t="e">
+        <f>AVERAGEIF(CImplData!$C:$C,A12,CImplData!$F:$F)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E12" t="str">
+        <f>LOOKUP($A12,CImplData!$C:$C,CImplData!$A:$A)</f>
+        <v>#FF00FFFF</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="str">
+        <f>LOOKUP($A13,CImplData!$C:$C,CImplData!B:B)</f>
+        <v>Resampling</v>
+      </c>
+      <c r="C13">
+        <f>COUNTIF(CImplData!$C:$C, $A13)</f>
+        <v>0</v>
+      </c>
+      <c r="D13" t="e">
+        <f>AVERAGEIF(CImplData!$C:$C,A13,CImplData!$F:$F)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E13" t="str">
+        <f>LOOKUP($A13,CImplData!$C:$C,CImplData!$A:$A)</f>
+        <v>#FF00FFFF</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="str">
+        <f>LOOKUP($A14,CImplData!$C:$C,CImplData!B:B)</f>
+        <v>Resampling</v>
+      </c>
+      <c r="C14">
+        <f>COUNTIF(CImplData!$C:$C, $A14)</f>
+        <v>0</v>
+      </c>
+      <c r="D14" t="e">
+        <f>AVERAGEIF(CImplData!$C:$C,A14,CImplData!$F:$F)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E14" t="str">
+        <f>LOOKUP($A14,CImplData!$C:$C,CImplData!$A:$A)</f>
+        <v>#FF00FFFF</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E14"/>
     </sheetView>
   </sheetViews>
@@ -54469,6 +54469,7 @@
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>